<commit_message>
Update subject, add/update chapter, import list teachers, delete user
</commit_message>
<xml_diff>
--- a/public/assets/templates/import_student_account_list.xlsx
+++ b/public/assets/templates/import_student_account_list.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53DE3F8-5F2A-47AC-819B-9A599612F518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9BB0E4-9136-4CA9-918E-E01C7E9873A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="88">
   <si>
-    <t>MSSV</t>
-  </si>
-  <si>
     <t>MatKhau</t>
   </si>
   <si>
@@ -285,6 +282,9 @@
   </si>
   <si>
     <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>MSSV/MSGV</t>
   </si>
 </sst>
 </file>
@@ -627,373 +627,373 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" customWidth="1"/>
-    <col min="3" max="3" width="31.36328125" customWidth="1"/>
-    <col min="4" max="4" width="18.81640625" customWidth="1"/>
-    <col min="5" max="5" width="19.08984375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="E6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="E7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="E8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>36</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>41</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>42</v>
       </c>
-      <c r="E10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>45</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>46</v>
       </c>
-      <c r="E11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>47</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>48</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>49</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>50</v>
       </c>
-      <c r="E12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>51</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>52</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>53</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>54</v>
       </c>
-      <c r="E13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>55</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>56</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>57</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>58</v>
       </c>
-      <c r="E14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>59</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>60</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>61</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>62</v>
       </c>
-      <c r="E15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>63</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>64</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>65</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>66</v>
       </c>
-      <c r="E16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>67</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>68</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>69</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>70</v>
       </c>
-      <c r="E17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>71</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>72</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>73</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>74</v>
       </c>
-      <c r="E18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>75</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>76</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>77</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>78</v>
       </c>
-      <c r="E19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>79</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>80</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>81</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>82</v>
       </c>
-      <c r="E20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>83</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>84</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>85</v>
       </c>
-      <c r="D21" t="s">
-        <v>86</v>
-      </c>
       <c r="E21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1029,19 +1029,19 @@
       <selection activeCell="I30" sqref="I30:I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.90625" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>